<commit_message>
add  file and update locations in code to read from it
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,17 +397,17 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.68359375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -438,7 +438,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -449,7 +449,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -460,7 +460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -471,7 +471,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -482,7 +482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
remove deprecated method and instance variable, add variables for multiple curfew times & write all to spreadsheet, move clock classes into separate files
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Bunk</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Late</t>
   </si>
   <si>
-    <t>Ozeret</t>
-  </si>
-  <si>
-    <t>Curfew</t>
-  </si>
-  <si>
     <t>Bunk 1</t>
   </si>
   <si>
@@ -74,6 +68,15 @@
   </si>
   <si>
     <t>Staff Member 4 ID</t>
+  </si>
+  <si>
+    <t>Normal Curfew</t>
+  </si>
+  <si>
+    <t>Night Off Curfew</t>
+  </si>
+  <si>
+    <t>Day Off Curfew</t>
   </si>
 </sst>
 </file>
@@ -109,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -394,20 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:G9"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.68359375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,76 +431,88 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add key sheet to spreadsheet, add method to read staff from it and create new StaffMember objects in a tracking arraylist
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,10 +5,11 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
+    <sheet name="Key" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Bunk</t>
   </si>
@@ -400,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,4 +518,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add inital sign out capability
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Bunk</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Day Off Curfew</t>
+  </si>
+  <si>
+    <t>Bunk 3</t>
+  </si>
+  <si>
+    <t>Staff Member 5</t>
+  </si>
+  <si>
+    <t>Staff Member 5 ID</t>
   </si>
 </sst>
 </file>
@@ -401,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +598,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change "normal curfew" to "leaving camp" curfew
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -71,9 +71,6 @@
     <t>Staff Member 4 ID</t>
   </si>
   <si>
-    <t>Normal Curfew</t>
-  </si>
-  <si>
     <t>Night Off Curfew</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>Staff Member 5 ID</t>
+  </si>
+  <si>
+    <t>Leaving Camp Curfew</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +443,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -454,7 +454,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -465,7 +465,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -600,13 +600,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change 'sign in' to 'sign in/out'
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Bunk</t>
   </si>
@@ -87,12 +87,28 @@
   </si>
   <si>
     <t>Leaving Camp Curfew</t>
+  </si>
+  <si>
+    <t>03/30/2022</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>12:55 PM (1:00 AM)</t>
+  </si>
+  <si>
+    <t>12:58 PM (5:00 PM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,12 +118,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,12 +158,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,17 +449,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="5.7109375" collapsed="true"/>
+    <col min="8" max="8" width="19.01953125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -439,6 +481,9 @@
       </c>
       <c r="G1" t="s">
         <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -451,6 +496,9 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -462,6 +510,9 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -473,6 +524,9 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -506,16 +560,28 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H9" t="s" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H10" t="s" s="6">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -539,8 +605,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
allow bunk column to also be titled 'position,' add initial code to move summary statistics to key sheet
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Bunk</t>
   </si>
@@ -102,13 +102,18 @@
   </si>
   <si>
     <t>12:58 PM (5:00 PM)</t>
+  </si>
+  <si>
+    <t>04/10/2022</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,23 +131,8 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
+        <fgColor rgb="FFB7E1CD"/>
       </patternFill>
     </fill>
   </fills>
@@ -158,17 +148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,23 +436,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="8" max="8" width="19.01953125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -485,50 +473,62 @@
       <c r="H1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -550,7 +550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -560,14 +560,14 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H9" t="s" s="3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -577,10 +577,10 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H10" t="s" s="6">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -599,14 +599,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="false"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
redesign spreadsheet to (1) move summary statistics to key sheet, (2) add daily summary to daily sheet (number of people who left camp, returned, are still out), and (3) made daily sheet into template to be copied for each day
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,11 +5,11 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <sheet name="Key" sheetId="2" r:id="rId2"/>
+    <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Bunk</t>
   </si>
@@ -89,25 +89,22 @@
     <t>Leaving Camp Curfew</t>
   </si>
   <si>
-    <t>03/30/2022</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>12:55 PM (1:00 AM)</t>
-  </si>
-  <si>
-    <t>12:58 PM (5:00 PM)</t>
-  </si>
-  <si>
-    <t>04/10/2022</t>
-  </si>
-  <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t># Left Camp</t>
+  </si>
+  <si>
+    <t># Returned to Camp</t>
+  </si>
+  <si>
+    <t># Still out of Camp</t>
+  </si>
+  <si>
+    <t>Time Out</t>
+  </si>
+  <si>
+    <t>Time In</t>
   </si>
 </sst>
 </file>
@@ -123,17 +120,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB7E1CD"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,11 +143,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,171 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,18 +442,32 @@
     <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -630,8 +477,11 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -641,8 +491,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -653,7 +506,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -664,7 +517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -678,4 +531,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6">
+        <f>COUNTA(A:A) - COUNTA(A1:A8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7">
+        <f>D6-D8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8">
+        <f>(COUNTIF(F:F, "=Day Off") + COUNTIF(F:F, "=Night Off") +  COUNTIF(F:F, "=Left Camp")) - (COUNTIF(F1:F8, "=Day Off") + COUNTIF(F1:F8, "=Night Off") +  COUNTIF(F1:F8, "=Left Camp"))</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
move summary statistics to key sheet, depracte 'todayCol' in favor of 'timeOutCol' and 'timeInCol,' add a new sheet named for today's date for each day, refactor 'getMasterStaffList()' to work with new spreadsheet formatting, depreacte 'readheaderRow()' in favor of new 'initializeAttendanceSheet()' that works with new spreadsheet formatting
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
-  <si>
-    <t>Bunk</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -128,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -136,20 +133,144 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,56 +551,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -488,44 +620,30 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -535,103 +653,117 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="H6" s="16"/>
+      <c r="I6" s="6">
+        <f>COUNTA(B:B) - COUNTA(B1:B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6">
-        <f>COUNTA(A:A) - COUNTA(A1:A8)</f>
+      <c r="H7" s="16"/>
+      <c r="I7" s="6">
+        <f>I6-I8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7">
-        <f>D6-D8</f>
+      <c r="H8" s="14"/>
+      <c r="I8" s="7">
+        <f>(COUNTIF(E:E, "=Day Off") + COUNTIF(E:E, "=Night Off") +  COUNTIF(E:E, "=Left Camp")) - (COUNTIF(E1:E8, "=Day Off") + COUNTIF(E1:E8, "=Night Off") +  COUNTIF(E1:E8, "=Left Camp"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8">
-        <f>(COUNTIF(F:F, "=Day Off") + COUNTIF(F:F, "=Night Off") +  COUNTIF(F:F, "=Left Camp")) - (COUNTIF(F1:F8, "=Day Off") + COUNTIF(F1:F8, "=Night Off") +  COUNTIF(F1:F8, "=Left Camp"))</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
+  <mergeCells count="7">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
set time out column to current time on sign out, set time in column to an indicator of how staff member signed outg
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -8,8 +8,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
+    <sheet name="04-13-2022" sheetId="3" r:id="rId1"/>
+    <sheet name="Key" sheetId="2" r:id="rId2"/>
+    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -102,6 +103,12 @@
   </si>
   <si>
     <t>Time In</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
   </si>
 </sst>
 </file>
@@ -551,9 +558,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="6">
+        <f>COUNTA(B:B) - COUNTA(B1:B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="6">
+        <f>I6-I8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="7">
+        <f>(COUNTIF(E:E, "=Day Off") + COUNTIF(E:E, "=Night Off") +  COUNTIF(E:E, "=Leaving Camp")) - (COUNTIF(E1:E8, "=Day Off") + COUNTIF(E1:E8, "=Night Off") +  COUNTIF(E1:E8, "=Left Camp"))</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -651,7 +782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>

</xml_diff>

<commit_message>
add signedOut/signedIn flags to StaffMember class, move left/returned/out calculation from spreadsheet to code, add additional null checks for cells, set timeInCol to be colored on sign out, move first written row up to newly open row, make aving resize all columns
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,12 +5,11 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="04-13-2022" sheetId="3" r:id="rId1"/>
-    <sheet name="Key" sheetId="2" r:id="rId2"/>
-    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
+    <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -103,12 +102,6 @@
   </si>
   <si>
     <t>Time In</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
   </si>
 </sst>
 </file>
@@ -558,10 +551,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="10.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,8 +663,7 @@
     <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
     <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -597,9 +690,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="18"/>
-      <c r="I2" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
@@ -608,9 +699,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="16"/>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
@@ -619,9 +708,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="14"/>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
@@ -637,10 +724,7 @@
         <v>22</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="6">
-        <f>COUNTA(B:B) - COUNTA(B1:B8)</f>
-        <v>0</v>
-      </c>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
@@ -649,10 +733,7 @@
         <v>23</v>
       </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="6">
-        <f>I6-I8</f>
-        <v>0</v>
-      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
@@ -662,231 +743,12 @@
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="7">
-        <f>(COUNTIF(E:E, "=Day Off") + COUNTIF(E:E, "=Night Off") +  COUNTIF(E:E, "=Leaving Camp")) - (COUNTIF(E1:E8, "=Day Off") + COUNTIF(E1:E8, "=Night Off") +  COUNTIF(E1:E8, "=Left Camp"))</f>
+        <f>I6-I7</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="6">
-        <f>COUNTA(B:B) - COUNTA(B1:B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="6">
-        <f>I6-I8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="7">
-        <f>(COUNTIF(E:E, "=Day Off") + COUNTIF(E:E, "=Night Off") +  COUNTIF(E:E, "=Left Camp")) - (COUNTIF(E1:E8, "=Day Off") + COUNTIF(E1:E8, "=Night Off") +  COUNTIF(E1:E8, "=Left Camp"))</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G5:H5"/>

</xml_diff>

<commit_message>
set up summary statistics on key sheet to function properly, make it so that curfew selection matters on signing out, not when signing in
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -554,14 +554,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D2" sqref="D2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -655,7 +658,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove deprecated todayCol variable, ensure that searches for staff look at only rows with staff in them, reevaluate formulas in spreadsheet upon saving, update signedOutList to work with new spreadsheet format,
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change staffList List to HashMap, change visitor sign out to actually sign them in, repalce stillOut excel formula with code, update correct row on keySheet with attendance stats, make some updates to sign in for visitors
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,15 +5,16 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="04-15-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -102,12 +103,25 @@
   </si>
   <si>
     <t>Time In</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>2:42 PM</t>
+  </si>
+  <si>
+    <t>Visitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,15 +131,35 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -233,11 +267,14 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -271,6 +308,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,18 +593,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -611,7 +651,9 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -646,6 +688,9 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -657,16 +702,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -745,10 +790,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="14"/>
-      <c r="I8" s="7">
-        <f>I6-I7</f>
-        <v>0</v>
-      </c>
+      <c r="I8" s="7"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -764,4 +806,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="8.484375" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="21">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s" s="20">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="7"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="7">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update some TODOs, add autosave to new sign in handler
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -818,13 +818,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="8.484375" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.3125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
implement helper methods for new sign in handler
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,16 +5,15 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="04-15-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -103,25 +102,12 @@
   </si>
   <si>
     <t>Time In</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>2:42 PM</t>
-  </si>
-  <si>
-    <t>Visitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,35 +117,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -267,14 +233,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -308,9 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -651,9 +611,7 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -688,9 +646,6 @@
       </c>
       <c r="C6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -702,16 +657,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -806,135 +761,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.3125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.484375" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s" s="20">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="7"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="7">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
set initial value of staffRowNum based on what currently exists in the spreadsheet instead of always to 1
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,11 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="04-20-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -102,12 +103,28 @@
   </si>
   <si>
     <t>Time In</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>10:12 PM</t>
+  </si>
+  <si>
+    <t>Leaving Camp</t>
+  </si>
+  <si>
+    <t>10:13 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,15 +134,35 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -233,11 +270,14 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -271,6 +311,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,12 +605,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -663,10 +709,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -761,4 +807,150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="21">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s" s="20">
+        <v>30</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s" s="23">
+        <v>30</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="7" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="7">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor save and exit button to use staffList HashMap
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,12 +9,11 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="04-20-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -103,28 +102,12 @@
   </si>
   <si>
     <t>Time In</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>10:12 PM</t>
-  </si>
-  <si>
-    <t>Leaving Camp</t>
-  </si>
-  <si>
-    <t>10:13 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,35 +117,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -270,14 +233,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -311,12 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,17 +554,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -709,10 +663,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -807,150 +761,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s" s="20">
-        <v>30</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="24">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s" s="23">
-        <v>30</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="6" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="7" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="7">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug of leaving a blank row above writing staff
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -554,7 +554,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
UI redesign (swapped locations of some buttons)
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,11 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="04-21-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -102,12 +103,43 @@
   </si>
   <si>
     <t>Time In</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>12:10 PM</t>
+  </si>
+  <si>
+    <t>Leaving Camp</t>
+  </si>
+  <si>
+    <t>12:12 PM</t>
+  </si>
+  <si>
+    <t>Night Off</t>
+  </si>
+  <si>
+    <t>Day Off</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>12:22 PM</t>
+  </si>
+  <si>
+    <t>12:26 PM (visitor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,15 +149,55 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -233,11 +305,14 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -271,6 +346,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,12 +650,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -597,7 +688,9 @@
       <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="n">
+        <v>1.0</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
@@ -663,10 +756,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -761,4 +854,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="9.6015625" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="9.6015625" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="21">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s" s="32">
+        <v>35</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="24">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s" s="23">
+        <v>32</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="27">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s" s="25">
+        <v>33</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="29">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="34">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="6" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="7" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="7">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
make save and restart button functional
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,16 +5,15 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="04-21-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -103,43 +102,12 @@
   </si>
   <si>
     <t>Time In</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>12:10 PM</t>
-  </si>
-  <si>
-    <t>Leaving Camp</t>
-  </si>
-  <si>
-    <t>12:12 PM</t>
-  </si>
-  <si>
-    <t>Night Off</t>
-  </si>
-  <si>
-    <t>Day Off</t>
-  </si>
-  <si>
-    <t>Visitor</t>
-  </si>
-  <si>
-    <t>12:22 PM</t>
-  </si>
-  <si>
-    <t>12:26 PM (visitor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,55 +117,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -305,14 +233,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -346,22 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,18 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -688,8 +597,8 @@
       <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>1.0</v>
+      <c r="D2" s="1">
+        <v>1</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -750,16 +659,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -854,180 +763,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" customWidth="true" width="9.6015625" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="9.6015625" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s" s="32">
-        <v>35</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="24">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s" s="23">
-        <v>32</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s" s="27">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s" s="25">
-        <v>33</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s" s="29">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s" s="34">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="6" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="6" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="7" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="7">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
track number of visitors on camp, summary stats now read 0 instead of blank
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -74,15 +74,6 @@
     <t>Day Off Curfew</t>
   </si>
   <si>
-    <t>Bunk 3</t>
-  </si>
-  <si>
-    <t>Staff Member 5</t>
-  </si>
-  <si>
-    <t>Staff Member 5 ID</t>
-  </si>
-  <si>
     <t>Leaving Camp Curfew</t>
   </si>
   <si>
@@ -102,6 +93,24 @@
   </si>
   <si>
     <t>Time In</t>
+  </si>
+  <si>
+    <t># Visitors on Camp</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>Visitor 1</t>
+  </si>
+  <si>
+    <t>Visitor 1 ID</t>
+  </si>
+  <si>
+    <t>Visitor 2</t>
+  </si>
+  <si>
+    <t>Visitor 2 ID</t>
   </si>
 </sst>
 </file>
@@ -125,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -233,11 +242,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -253,6 +299,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,11 +604,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -569,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -597,9 +648,7 @@
       <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
@@ -641,13 +690,24 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -657,10 +717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -682,83 +742,92 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="18"/>
+      <c r="G2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="21"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="17"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="16"/>
+      <c r="G6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="19"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="16"/>
+      <c r="G7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="19"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="7"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
onCampList shows all staff on camp now
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,11 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="04-29-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -111,12 +112,36 @@
   </si>
   <si>
     <t>Visitor 2 ID</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>4:27 PM</t>
+  </si>
+  <si>
+    <t>Leaving
+Camp</t>
+  </si>
+  <si>
+    <t>4:29 PM</t>
+  </si>
+  <si>
+    <t>Leaving 
+Camp</t>
+  </si>
+  <si>
+    <t>4:30 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,15 +151,55 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -279,11 +344,14 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -324,6 +392,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,12 +687,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -686,6 +763,9 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -725,10 +805,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -832,4 +912,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="8.484375" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s" s="23">
+        <v>33</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="27">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s" s="28">
+        <v>36</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="6" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add warning if no curfew time radio button was selected
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,16 +5,15 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="04-29-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -112,36 +111,12 @@
   </si>
   <si>
     <t>Visitor 2 ID</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>4:27 PM</t>
-  </si>
-  <si>
-    <t>Leaving
-Camp</t>
-  </si>
-  <si>
-    <t>4:29 PM</t>
-  </si>
-  <si>
-    <t>Leaving 
-Camp</t>
-  </si>
-  <si>
-    <t>4:30 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,55 +126,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -344,14 +279,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -368,10 +300,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -380,27 +318,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,16 +606,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -763,9 +688,6 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,16 +721,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -831,70 +753,70 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="19"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="15"/>
+      <c r="H10" s="21"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>
@@ -912,165 +834,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" customWidth="true" width="8.484375" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s" s="23">
-        <v>33</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="27">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s" s="28">
-        <v>36</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="6" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="6" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="7" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="13" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="8">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
software now reads from today's sheet if it exists and starts with internal data in same state as today's sheet reads
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,11 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
+    <sheet name="05-03-2022" sheetId="3" r:id="rId2"/>
+    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -111,12 +112,35 @@
   </si>
   <si>
     <t>Visitor 2 ID</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>10:02 PM</t>
+  </si>
+  <si>
+    <t>10:03 PM</t>
+  </si>
+  <si>
+    <t>Day 
+Off</t>
+  </si>
+  <si>
+    <t>10:40 PM</t>
+  </si>
+  <si>
+    <t>10:40 PM (visitor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,15 +150,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -279,11 +333,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -300,6 +363,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,6 +393,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,17 +681,17 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+      <selection activeCell="D2" sqref="D2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -650,7 +724,9 @@
       <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="n">
+        <v>1.0</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
@@ -722,15 +798,180 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.6015625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.6015625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="19">
+        <v>0.92013888888888884</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="6" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="6" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -753,70 +994,70 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="19"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
program now reads from yesterday's sheet and writes people who are still out of camp in to be taken care of today
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,10 +5,11 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="05-04-2022" r:id="rId7" sheetId="4"/>
     <sheet name="05-03-2022" sheetId="3" r:id="rId2"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -120,20 +121,25 @@
     <t>5:00 PM</t>
   </si>
   <si>
-    <t>10:02 PM</t>
-  </si>
-  <si>
-    <t>10:03 PM</t>
+    <t>7:05 PM</t>
+  </si>
+  <si>
+    <t>Leaving 
+Camp</t>
+  </si>
+  <si>
+    <t>Night 
+Off</t>
   </si>
   <si>
     <t>Day 
 Off</t>
   </si>
   <si>
-    <t>10:40 PM</t>
-  </si>
-  <si>
-    <t>10:40 PM (visitor)</t>
+    <t>7:06 PM</t>
+  </si>
+  <si>
+    <t>Yesterday (7:05 PM)</t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,27 +174,22 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="B7E1CD"/>
+        <fgColor rgb="FFB7E1CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
+        <fgColor rgb="00A7E1"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -342,11 +343,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -363,12 +367,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,11 +401,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,12 +701,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -724,8 +739,8 @@
       <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>1.0</v>
+      <c r="D2" s="1">
+        <v>2</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -764,6 +779,9 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -798,18 +816,18 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.6015625" collapsed="true"/>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.6015625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -831,24 +849,24 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="19">
-        <v>0.92013888888888884</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="E2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
@@ -858,92 +876,127 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0.9194444444444444</v>
-      </c>
-      <c r="G4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="25"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G6" s="20" t="s">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="6" t="n">
-        <v>2.0</v>
+      <c r="H6" s="27"/>
+      <c r="I6" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="22" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="6" t="n">
-        <v>2.0</v>
+      <c r="H7" s="27"/>
+      <c r="I7" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="24" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="7" t="n">
-        <v>0.0</v>
+      <c r="H8" s="29"/>
+      <c r="I8" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="13" t="n">
-        <v>0.0</v>
+      <c r="H10" s="31"/>
+      <c r="I10" s="13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G3:H3"/>
@@ -994,70 +1047,70 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="25"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="25"/>
+      <c r="H8" s="29"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>
@@ -1075,4 +1128,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="34">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s" s="33">
+        <v>33</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="37">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s" s="36">
+        <v>34</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="40">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s" s="39">
+        <v>35</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="43">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="42">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="6" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="7" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="13" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update code to use CurfewType, allow people to sign in/out multiple times in one day
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -122,14 +122,6 @@
   </si>
   <si>
     <t>7:05 PM</t>
-  </si>
-  <si>
-    <t>Leaving 
-Camp</t>
-  </si>
-  <si>
-    <t>Night 
-Off</t>
   </si>
   <si>
     <t>Day 
@@ -140,6 +132,12 @@
   </si>
   <si>
     <t>Yesterday (7:05 PM)</t>
+  </si>
+  <si>
+    <t>10:47 PM</t>
+  </si>
+  <si>
+    <t>10:48 PM</t>
   </si>
 </sst>
 </file>
@@ -156,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,12 +178,27 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor rgb="00A7E1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
       </patternFill>
     </fill>
   </fills>
@@ -350,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -367,15 +380,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -401,18 +413,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,12 +710,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -742,7 +751,9 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="n">
+        <v>1.0</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -755,7 +766,9 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -768,6 +781,12 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,7 +835,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,19 +873,19 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="E2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
@@ -878,19 +897,19 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
@@ -902,19 +921,19 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="28" t="s">
+      <c r="E4" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="29"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="9" t="s">
         <v>31</v>
       </c>
@@ -926,17 +945,17 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -946,19 +965,19 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="6">
         <v>4</v>
       </c>
@@ -966,37 +985,36 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="31"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="13">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G3:H3"/>
@@ -1008,6 +1026,7 @@
     <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1047,70 +1066,70 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="29"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="31"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>
@@ -1140,11 +1159,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="9.6015625" collapsed="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1166,135 +1187,122 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="34">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s" s="33">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s" s="31">
         <v>33</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="37">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s" s="36">
-        <v>34</v>
-      </c>
-      <c r="G3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s" s="34">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s" s="33">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="40">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="37">
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
       </c>
       <c r="E4" t="s" s="39">
-        <v>35</v>
-      </c>
-      <c r="G4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="29"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s" s="43">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s" s="42">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="31"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="13" t="n">
         <v>1.0</v>
       </c>

</xml_diff>

<commit_message>
make sure additional windows not needing to open doesn't overwrite sign-in confirmation text
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,8 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-04-2022" r:id="rId7" sheetId="4"/>
-    <sheet name="05-03-2022" sheetId="3" r:id="rId2"/>
+    <sheet name="05-05-2022" r:id="rId7" sheetId="4"/>
+    <sheet name="05-04-2022" sheetId="3" r:id="rId2"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -134,10 +134,35 @@
     <t>Yesterday (7:05 PM)</t>
   </si>
   <si>
-    <t>10:47 PM</t>
-  </si>
-  <si>
-    <t>10:48 PM</t>
+    <t>11:41 AM</t>
+  </si>
+  <si>
+    <t>11:42 AM</t>
+  </si>
+  <si>
+    <t>11:45 AM</t>
+  </si>
+  <si>
+    <t>11:47 AM</t>
+  </si>
+  <si>
+    <t>11:49 AM</t>
+  </si>
+  <si>
+    <t>Night 
+Off</t>
+  </si>
+  <si>
+    <t>11:50 AM</t>
+  </si>
+  <si>
+    <t>11:53 AM</t>
+  </si>
+  <si>
+    <t>6:51 PM (visitor)</t>
+  </si>
+  <si>
+    <t>6:52 PM</t>
   </si>
 </sst>
 </file>
@@ -168,11 +193,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
       </patternFill>
     </fill>
@@ -182,8 +202,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
       </patternFill>
     </fill>
     <fill>
@@ -201,6 +221,11 @@
         <fgColor rgb="FFE599"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -363,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -380,15 +405,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,15 +433,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +740,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,12 +783,8 @@
       <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1.0</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -766,8 +797,8 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
+      <c r="D3" s="1" t="n">
+        <v>1.0</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -782,11 +813,11 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,8 +830,8 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,7 +866,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,150 +899,105 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="23" t="s">
+      <c r="E2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="E3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="26"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="27" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="28"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="28"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1066,70 +1052,70 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="26"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="28"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="28"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>
@@ -1159,13 +1145,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.1484375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.73828125" collapsed="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="9.6015625" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.73828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1192,43 +1178,43 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="32">
+      <c r="C2" t="s" s="27">
         <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s" s="31">
-        <v>33</v>
-      </c>
-      <c r="G2" s="23" t="s">
+      <c r="E2" t="s" s="28">
+        <v>36</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s" s="34">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s" s="33">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="32">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s" s="34">
+        <v>39</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="26"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1238,73 +1224,99 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s" s="37">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s" s="39">
-        <v>37</v>
-      </c>
-      <c r="G4" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s" s="38">
+        <v>42</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="28"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="42">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s" s="48">
+        <v>45</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="25" t="s">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s" s="44">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="47">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="6" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="6" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="28"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update daily tracking numbers so as to not count same staff member multiple times
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -134,35 +134,16 @@
     <t>Yesterday (7:05 PM)</t>
   </si>
   <si>
-    <t>11:41 AM</t>
-  </si>
-  <si>
-    <t>11:42 AM</t>
-  </si>
-  <si>
-    <t>11:45 AM</t>
-  </si>
-  <si>
-    <t>11:47 AM</t>
-  </si>
-  <si>
-    <t>11:49 AM</t>
-  </si>
-  <si>
-    <t>Night 
-Off</t>
-  </si>
-  <si>
-    <t>11:50 AM</t>
-  </si>
-  <si>
-    <t>11:53 AM</t>
-  </si>
-  <si>
-    <t>6:51 PM (visitor)</t>
-  </si>
-  <si>
-    <t>6:52 PM</t>
+    <t>Yesterday (7:06 PM)</t>
+  </si>
+  <si>
+    <t>6:59 PM (visitor)</t>
+  </si>
+  <si>
+    <t>6:59 PM</t>
+  </si>
+  <si>
+    <t>7:00 PM</t>
   </si>
 </sst>
 </file>
@@ -170,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +159,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +188,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FF00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -221,11 +225,6 @@
         <fgColor rgb="FFE599"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -385,10 +384,11 @@
       <right style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -409,6 +409,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,32 +435,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,8 +788,8 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>1.0</v>
+      <c r="D3" s="1">
+        <v>1</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -814,10 +805,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,8 +821,8 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="n">
-        <v>2.0</v>
+      <c r="D5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,7 +857,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,10 +904,10 @@
       <c r="E2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
@@ -937,21 +928,34 @@
       <c r="E3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="22" t="s">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="9" t="s">
         <v>31</v>
       </c>
@@ -959,45 +963,45 @@
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1052,70 +1056,70 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>
@@ -1145,13 +1149,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.1484375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.73828125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.73828125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1178,145 +1182,132 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="27">
+      <c r="C2" t="s" s="29">
         <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s" s="28">
-        <v>36</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="E2" t="s" s="33">
+        <v>38</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s" s="32">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s" s="31">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s" s="32">
         <v>37</v>
       </c>
-      <c r="E3" t="s" s="34">
-        <v>39</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s" s="37">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s" s="38">
-        <v>42</v>
-      </c>
-      <c r="G4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s" s="36">
+        <v>33</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s" s="42">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s" s="48">
-        <v>45</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="39">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="38">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s" s="44">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s" s="47">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="20" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="6" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
decrement on-time count when a staff member signs out again after previously signing in
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,12 +5,12 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-05-2022" r:id="rId7" sheetId="4"/>
-    <sheet name="05-04-2022" sheetId="3" r:id="rId2"/>
+    <sheet name="05-06-2022" r:id="rId7" sheetId="4"/>
+    <sheet name="05-05-2022" sheetId="3" r:id="rId2"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -135,15 +135,6 @@
   </si>
   <si>
     <t>Yesterday (7:06 PM)</t>
-  </si>
-  <si>
-    <t>6:59 PM (visitor)</t>
-  </si>
-  <si>
-    <t>6:59 PM</t>
-  </si>
-  <si>
-    <t>7:00 PM</t>
   </si>
 </sst>
 </file>
@@ -388,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -439,12 +430,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
   </cellXfs>
@@ -730,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,9 +776,7 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -805,10 +791,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -820,9 +803,6 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1188,8 +1168,8 @@
       <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s" s="33">
-        <v>38</v>
+      <c r="E2" t="s" s="32">
+        <v>31</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>17</v>
@@ -1209,8 +1189,8 @@
       <c r="C3" t="s" s="31">
         <v>27</v>
       </c>
-      <c r="D3" t="s" s="32">
-        <v>37</v>
+      <c r="D3" t="s" s="30">
+        <v>25</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -1230,13 +1210,13 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="37">
+      <c r="C4" t="s" s="36">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s" s="36">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s" s="35">
         <v>33</v>
       </c>
       <c r="G4" s="24" t="s">
@@ -1248,21 +1228,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s" s="39">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s" s="38">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
       <c r="I5" s="8"/>

</xml_diff>

<commit_message>
add more comments to config.ini, make rolloverTime optional, combine EventHandlers for saveAndExit, saveAndRestart, rollover into a single handler to minimize repeated code
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,13 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-06-2022" r:id="rId7" sheetId="4"/>
     <sheet name="05-05-2022" sheetId="3" r:id="rId2"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -129,19 +128,12 @@
   </si>
   <si>
     <t>7:06 PM</t>
-  </si>
-  <si>
-    <t>Yesterday (7:05 PM)</t>
-  </si>
-  <si>
-    <t>Yesterday (7:06 PM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,33 +183,8 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -371,15 +338,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -426,15 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -724,12 +679,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -789,9 +744,6 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -842,13 +794,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,10 +962,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1117,178 +1069,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false">
-      <selection activeCell="P5" sqref="P5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s" s="29">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s" s="32">
-        <v>31</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s" s="31">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s" s="30">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="36">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s" s="35">
-        <v>33</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="6" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="6" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="7" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="13" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="8">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add a second day off curfew to make sure people who are on the first and second day of their days off are treated correctly
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -9,12 +9,13 @@
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-05-2022" sheetId="3" r:id="rId2"/>
+    <sheet name="05-07-2022" r:id="rId7" sheetId="4"/>
+    <sheet name="05-06-2022" sheetId="3" r:id="rId2"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -128,12 +129,28 @@
   </si>
   <si>
     <t>7:06 PM</t>
+  </si>
+  <si>
+    <t>Yesterday (7:05 PM)</t>
+  </si>
+  <si>
+    <t>Yesterday (7:06 PM)</t>
+  </si>
+  <si>
+    <t>1:24 PM</t>
+  </si>
+  <si>
+    <t>1:22 PM</t>
+  </si>
+  <si>
+    <t>1:26 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +200,33 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -338,12 +380,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -390,6 +435,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -679,12 +735,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -745,6 +801,9 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -755,6 +814,9 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,13 +856,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -962,10 +1024,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1069,4 +1131,178 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="29">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s" s="36">
+        <v>39</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s" s="31">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s" s="30">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="34">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s" s="37">
+        <v>39</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="6" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="6" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="13" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
replace offCampList alert window with actual popup to sign people in
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,17 +5,16 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-07-2022" r:id="rId7" sheetId="4"/>
     <sheet name="05-06-2022" sheetId="3" r:id="rId2"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -129,28 +128,12 @@
   </si>
   <si>
     <t>7:06 PM</t>
-  </si>
-  <si>
-    <t>Yesterday (7:05 PM)</t>
-  </si>
-  <si>
-    <t>Yesterday (7:06 PM)</t>
-  </si>
-  <si>
-    <t>1:24 PM</t>
-  </si>
-  <si>
-    <t>1:22 PM</t>
-  </si>
-  <si>
-    <t>1:26 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,33 +183,8 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -380,15 +338,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -435,17 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -729,18 +673,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.44921875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -801,8 +745,11 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="n">
-        <v>1.0</v>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,8 +762,8 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="n">
-        <v>1.0</v>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,19 +797,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1024,10 +971,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1131,178 +1078,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="false">
-      <selection activeCell="P5" sqref="P5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="17.44921875" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="19.1484375" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s" s="29">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s" s="36">
-        <v>39</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s" s="31">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s" s="30">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="34">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s" s="37">
-        <v>39</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="6" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="6" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="7" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="13" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="8">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
replace onCampList alert window with actual popup to sign people out, add styling for popup to make it look like a true dropdown
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,12 +5,11 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-06-2022" sheetId="3" r:id="rId2"/>
-    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId3"/>
+    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -57,18 +56,6 @@
     <t>Staff Member 4</t>
   </si>
   <si>
-    <t>Staff Member 1 ID</t>
-  </si>
-  <si>
-    <t>Staff Member 2 ID</t>
-  </si>
-  <si>
-    <t>Staff Member 3 ID</t>
-  </si>
-  <si>
-    <t>Staff Member 4 ID</t>
-  </si>
-  <si>
     <t>Night Off Curfew</t>
   </si>
   <si>
@@ -105,36 +92,32 @@
     <t>Visitor 1</t>
   </si>
   <si>
-    <t>Visitor 1 ID</t>
-  </si>
-  <si>
     <t>Visitor 2</t>
   </si>
   <si>
-    <t>Visitor 2 ID</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>7:05 PM</t>
-  </si>
-  <si>
-    <t>Day 
-Off</t>
-  </si>
-  <si>
-    <t>7:06 PM</t>
+    <t>S000001</t>
+  </si>
+  <si>
+    <t>S000002</t>
+  </si>
+  <si>
+    <t>S000003</t>
+  </si>
+  <si>
+    <t>S000004</t>
+  </si>
+  <si>
+    <t>V000001</t>
+  </si>
+  <si>
+    <t>V000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,49 +125,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -329,21 +279,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -360,12 +300,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,8 +325,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -673,15 +606,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -689,7 +622,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -715,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -729,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -743,13 +676,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,29 +687,26 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>29</v>
@@ -794,174 +718,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="13">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -979,7 +735,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -988,79 +744,79 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="21"/>
+      <c r="G2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="G3" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="23"/>
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="17"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="G4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="25"/>
+      <c r="G4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="19"/>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="G6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="23"/>
+      <c r="G6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="17"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="23"/>
+      <c r="G7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="G8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="25"/>
+      <c r="G8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="19"/>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="27"/>
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="21"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish updating README.md for current functionality
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,15 +5,16 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="05-07-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -111,12 +112,26 @@
   </si>
   <si>
     <t>V000002</t>
+  </si>
+  <si>
+    <t>1:00 AM</t>
+  </si>
+  <si>
+    <t>5:00 PM</t>
+  </si>
+  <si>
+    <t>8:28 PM</t>
+  </si>
+  <si>
+    <t>Leaving 
+Camp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,15 +141,35 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A7E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA999E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA999E"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -279,11 +314,14 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -324,6 +362,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,18 +656,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.9765625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -721,16 +771,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -834,4 +884,191 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" customWidth="true" width="8.296875" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="8.73828125" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s" s="23">
+        <v>33</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="27">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="30">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s" s="29">
+        <v>33</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="6" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="7" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update colors, fonts, and image from OSRUI to Harlam
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,16 +5,15 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="05-07-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -112,26 +111,12 @@
   </si>
   <si>
     <t>V000002</t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>5:00 PM</t>
-  </si>
-  <si>
-    <t>8:28 PM</t>
-  </si>
-  <si>
-    <t>Leaving 
-Camp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,35 +126,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A7E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA999E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA999E"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -314,14 +279,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -362,18 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,17 +610,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.9765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.05078125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.3125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -690,7 +640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -704,7 +654,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -718,7 +668,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -729,7 +679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -740,7 +690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -751,7 +701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -775,15 +725,15 @@
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.68359375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.68359375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.68359375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.68359375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -800,7 +750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="G2" s="14" t="s">
@@ -809,7 +759,7 @@
       <c r="H2" s="15"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="16" t="s">
@@ -818,7 +768,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="G4" s="18" t="s">
@@ -827,14 +777,14 @@
       <c r="H4" s="19"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="G6" s="16" t="s">
@@ -843,7 +793,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="G7" s="16" t="s">
@@ -852,7 +802,7 @@
       <c r="H7" s="17"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="18" t="s">
@@ -861,8 +811,8 @@
       <c r="H8" s="19"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="G10" s="20" t="s">
         <v>20</v>
       </c>
@@ -884,191 +834,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" customWidth="true" width="8.296875" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="8.73828125" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s" s="23">
-        <v>33</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="27">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s" s="26">
-        <v>33</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="30">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s" s="29">
-        <v>33</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s" s="33">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s" s="32">
-        <v>33</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="6" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="6" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="7" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="13" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="8">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add function to OzeretPane that lists everyone in the key sheet in today's sheet
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,15 +5,16 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="06-07-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -68,15 +69,6 @@
     <t>Position</t>
   </si>
   <si>
-    <t># Left Camp</t>
-  </si>
-  <si>
-    <t># Returned to Camp</t>
-  </si>
-  <si>
-    <t># Still out of Camp</t>
-  </si>
-  <si>
     <t>Time Out</t>
   </si>
   <si>
@@ -111,12 +103,34 @@
   </si>
   <si>
     <t>V000002</t>
+  </si>
+  <si>
+    <t># Left</t>
+  </si>
+  <si>
+    <t># Returned</t>
+  </si>
+  <si>
+    <t># Still Out</t>
+  </si>
+  <si>
+    <t>12:00 AM</t>
+  </si>
+  <si>
+    <t>12:30 AM</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Not in Bunk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,15 +140,25 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="EA9999"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -279,11 +303,14 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -324,6 +351,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,17 +649,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.05078125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.3125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -640,7 +679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -648,13 +687,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -662,13 +701,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -676,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -687,29 +726,29 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -722,18 +761,18 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.68359375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.68359375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.68359375" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="10.68359375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -744,13 +783,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="G2" s="14" t="s">
@@ -759,7 +798,7 @@
       <c r="H2" s="15"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="16" t="s">
@@ -768,7 +807,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="G4" s="18" t="s">
@@ -777,50 +816,49 @@
       <c r="H4" s="19"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="G6" s="16" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="G7" s="16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="18" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G10" s="20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="13"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G3:H3"/>
@@ -834,4 +872,214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="9.73828125" collapsed="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="23">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s" s="22">
+        <v>33</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="25">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s" s="24">
+        <v>33</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="27">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="29">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s" s="28">
+        <v>33</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s" s="31">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s" s="30">
+        <v>33</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="6" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s" s="33">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="7" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update ozeret-mode sign in button to work correctly with that mode
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -114,16 +114,19 @@
     <t># Still Out</t>
   </si>
   <si>
-    <t>12:00 AM</t>
-  </si>
-  <si>
-    <t>12:30 AM</t>
+    <t>9:55 PM</t>
+  </si>
+  <si>
+    <t>9:57 PM</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Not in Bunk</t>
+  </si>
+  <si>
+    <t>9:54 PM</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +160,26 @@
         <fgColor rgb="EA9999"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="B7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE599"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -310,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -363,6 +386,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,12 +678,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.9765625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -690,7 +717,9 @@
         <v>21</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -703,7 +732,9 @@
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -717,6 +748,9 @@
       <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -728,6 +762,9 @@
       <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -739,6 +776,9 @@
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D6" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -749,6 +789,9 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -884,11 +927,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" customWidth="true" width="11.51953125" collapsed="true" bestFit="true"/>
+    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="9.73828125" collapsed="true" bestFit="true"/>
+    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="8.9765625" collapsed="true" bestFit="true"/>
+    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" customWidth="true" width="8.484375" collapsed="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -921,8 +966,8 @@
       <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s" s="22">
-        <v>33</v>
+      <c r="E2" t="s" s="34">
+        <v>34</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>13</v>
@@ -969,8 +1014,8 @@
       <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s" s="26">
-        <v>33</v>
+      <c r="E4" t="s" s="36">
+        <v>34</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>12</v>
@@ -1045,7 +1090,7 @@
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1056,7 +1101,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="7" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updat README with new functionality added in version 2.1
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,16 +5,15 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="06-07-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -112,28 +111,12 @@
   </si>
   <si>
     <t># Still Out</t>
-  </si>
-  <si>
-    <t>9:55 PM</t>
-  </si>
-  <si>
-    <t>9:57 PM</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Not in Bunk</t>
-  </si>
-  <si>
-    <t>9:54 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,45 +126,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="EA9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="B7E1CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE599"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -326,14 +279,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -374,22 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,12 +612,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.9765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.84765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.3125" collapsed="true"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -716,7 +650,9 @@
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
@@ -776,8 +712,8 @@
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="n">
-        <v>2.0</v>
+      <c r="D6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -790,8 +726,8 @@
       <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="n">
-        <v>2.0</v>
+      <c r="D7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -809,10 +745,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="9" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -915,216 +851,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" customWidth="true" width="11.51953125" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
-    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="8.9765625" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
-    <col min="9" max="9" customWidth="true" width="8.484375" collapsed="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="23">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s" s="34">
-        <v>34</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="25">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s" s="24">
-        <v>33</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s" s="27">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s" s="36">
-        <v>34</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s" s="29">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s" s="28">
-        <v>33</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s" s="31">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s" s="30">
-        <v>33</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="6" t="n">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s" s="33">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s" s="32">
-        <v>33</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="6" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="7" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add ability to sign staff in on day off and shmira in ozeret mode, change ozeret mode 'day off' curfew to 'shabbat' curfew
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,11 +5,11 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
-    <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
+    <sheet name="Daily Attendance Template" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,12 +650,8 @@
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -668,9 +664,7 @@
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
@@ -684,9 +678,6 @@
       <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -698,9 +689,6 @@
       <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -712,9 +700,6 @@
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -725,9 +710,6 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -739,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add failsafe for getting needed sheets if the names aren't there
</commit_message>
<xml_diff>
--- a/resources/files/Sample_Attendance_File.xlsx
+++ b/resources/files/Sample_Attendance_File.xlsx
@@ -5,10 +5,12 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
+    <sheet name="06-22-2022" r:id="rId8" sheetId="5"/>
+    <sheet name="06-21-2022" r:id="rId7" sheetId="4"/>
     <sheet name="05-07-2022" r:id="rId6" sheetId="3"/>
     <sheet name="Daily Attendance Template" sheetId="1" r:id="rId2"/>
   </sheets>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -896,12 +898,322 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" customWidth="true" width="8.296875" collapsed="true" bestFit="true"/>
-    <col min="2" max="2" customWidth="true" width="15.04296875" collapsed="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.2578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.04296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.73828125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.3125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.296875" collapsed="true"/>
     <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="1" max="1" customWidth="true" width="8.2578125" collapsed="true" bestFit="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="8.73828125" collapsed="true" bestFit="true"/>
-    <col min="4" max="4" customWidth="true" width="9.3125" collapsed="true" bestFit="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s" s="23">
+        <v>33</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="27">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="30">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s" s="29">
+        <v>33</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="33">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s" s="32">
+        <v>33</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="6" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="7" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.62109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="G6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="10.7109375" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="8.62109375" collapsed="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -923,21 +1235,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s" s="23">
-        <v>33</v>
-      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="G2" s="14" t="s">
         <v>13</v>
       </c>
@@ -947,21 +1246,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="27">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s" s="26">
-        <v>33</v>
-      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="G3" s="16" t="s">
         <v>11</v>
       </c>
@@ -971,21 +1257,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="30">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s" s="29">
-        <v>33</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="G4" s="18" t="s">
         <v>12</v>
       </c>
@@ -995,21 +1268,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s" s="33">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s" s="32">
-        <v>33</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="8"/>
@@ -1021,9 +1281,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="17"/>
-      <c r="I6" s="6" t="n">
-        <v>4.0</v>
-      </c>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
@@ -1032,9 +1290,7 @@
         <v>16</v>
       </c>
       <c r="H7" s="17"/>
-      <c r="I7" s="6" t="n">
-        <v>0.0</v>
-      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
@@ -1043,9 +1299,7 @@
         <v>17</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="7" t="n">
-        <v>4.0</v>
-      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1053,9 +1307,7 @@
         <v>20</v>
       </c>
       <c r="H10" s="21"/>
-      <c r="I10" s="13" t="n">
-        <v>0.0</v>
-      </c>
+      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>